<commit_message>
updates to appl stock yearly earnings per share pie chart
</commit_message>
<xml_diff>
--- a/earnings_df.xlsx
+++ b/earnings_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C1EF5AE1F89797E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6367FF43-5E24-4108-BA16-EA22E50AB0CF}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C382DA813F1797E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADBEB6DB-ABF6-4419-BD8E-01AEDA61C371}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
developed msft yearly earnings pie chart
</commit_message>
<xml_diff>
--- a/earnings_df.xlsx
+++ b/earnings_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C23E5E8277F787E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B02F71D-06D1-416C-88A6-D9BDC4E93FE0}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4CE2EDAB21BB797E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57C5DEBA-A566-43EC-86B9-7A5B52019093}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
developed nflx yearly earnings pie chart
</commit_message>
<xml_diff>
--- a/earnings_df.xlsx
+++ b/earnings_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C4455E839A1797E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D52385B3-E297-4C28-B9D7-58D52406AEF6}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4CAF65E9023F797E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7228B0B3-F1A0-4765-8A21-66F5F4727643}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
developed pfe yearly earnings pie chart
</commit_message>
<xml_diff>
--- a/earnings_df.xlsx
+++ b/earnings_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4CC795693463797E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16C04866-6673-47C6-A2C4-8F11BA6600CC}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C7E0DEE1001797E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3801808-33EB-4751-9EDF-FB73E736096D}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
developed nke yearly earnings pie chart
</commit_message>
<xml_diff>
--- a/earnings_df.xlsx
+++ b/earnings_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C374D69199B797E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{467F455B-B5F8-4C4B-97CE-387F6EF76149}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4CDA9DEC2191787E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{155ED2BF-A750-416D-A66F-8EEE6CDE8B7F}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
created merge of msft and nflx yearly earnings per share
</commit_message>
<xml_diff>
--- a/earnings_df.xlsx
+++ b/earnings_df.xlsx
@@ -8,25 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_1F6182FCF6EB08120B2D4CA64D291E0D787E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B04349A9-C764-4841-A19A-D7E008854FBC}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C5DAD6C29FD797E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16F612A5-3D23-4C94-BB63-64627B4F1756}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1522,10 +1511,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1817,9 +1802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1782"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1830,7 +1813,6 @@
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
developed blue chip stocks yearly earnings per share df
</commit_message>
<xml_diff>
--- a/earnings_df.xlsx
+++ b/earnings_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4CD25528290F797E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F77D6BB5-8954-4220-869A-0C7C28695318}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4CED852F07D5797E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25EEF51F-4241-43B0-92CA-5ACD3066FEEB}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
confirming updates complete for negative yearly earnings per share 2012 dataframe
</commit_message>
<xml_diff>
--- a/earnings_df.xlsx
+++ b/earnings_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C9F05683007787E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB370AC3-8EA7-421E-AC4F-E2CA4D38AAFF}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C0F7DAD2EFB787E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5B0B945-3C3F-48CF-AB6C-563B37C59786}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
developed negative yearly earnings per share 2013 dataframe
</commit_message>
<xml_diff>
--- a/earnings_df.xlsx
+++ b/earnings_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C0F7DAD2EFB787E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5B0B945-3C3F-48CF-AB6C-563B37C59786}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C1BF5EB0881787E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8C2F043-CD55-423B-84D6-1541E996E6CD}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
developed negative yearly earnings per share 2014 dataframe
</commit_message>
<xml_diff>
--- a/earnings_df.xlsx
+++ b/earnings_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C1BF5EB0881787E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8C2F043-CD55-423B-84D6-1541E996E6CD}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C0C85E81C23797E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD1AAA44-5E20-431E-A247-01F7B1F00C5C}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
developed negative yearly earnings per share 2015 dataframe
</commit_message>
<xml_diff>
--- a/earnings_df.xlsx
+++ b/earnings_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C0C85E81C23797E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD1AAA44-5E20-431E-A247-01F7B1F00C5C}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C810DED2EA5787E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02FEEB5D-9BD2-4164-9E7B-A5EBA372E672}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
developed negative yearly earnings per share 2016 dataframe
</commit_message>
<xml_diff>
--- a/earnings_df.xlsx
+++ b/earnings_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C810DED2EA5787E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02FEEB5D-9BD2-4164-9E7B-A5EBA372E672}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C99B5EB2CED787E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D62B1AA-8449-41BF-82E5-A79CA6A98086}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
developed negative yearly earnings per share 2017 dataframe
</commit_message>
<xml_diff>
--- a/earnings_df.xlsx
+++ b/earnings_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C99B5EB2CED787E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D62B1AA-8449-41BF-82E5-A79CA6A98086}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1F6182FCF6EB08120B2D4C940DEC0BEB787E8300" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F747EA3-D92F-40EC-BAA1-F005A44A1547}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>